<commit_message>
Adjustments associated with removal of recombinant AAVs
</commit_message>
<xml_diff>
--- a/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/Parvoviridae-GLUE/tabular/references/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC1F8F-68E9-8B4D-AAB1-C9575E7F09D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1200" windowWidth="30860" windowHeight="25440" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1102,9 +1108,6 @@
     <t>virus_clade</t>
   </si>
   <si>
-    <t>AAV</t>
-  </si>
-  <si>
     <t>Reptile</t>
   </si>
   <si>
@@ -1112,12 +1115,15 @@
   </si>
   <si>
     <t>Nephroparvovirus</t>
+  </si>
+  <si>
+    <t>AAV_primate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1173,7 +1179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1264,6 +1270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEF3A8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2007,7 +2019,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2048,6 +2060,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="731">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2784,6 +2797,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3108,14 +3129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1048576"/>
+      <selection sqref="A1:G100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -3125,7 +3146,7 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3148,7 +3169,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -3168,7 +3189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
@@ -3188,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
         <v>16</v>
       </c>
@@ -3208,7 +3229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>96</v>
       </c>
@@ -3228,7 +3249,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>99</v>
       </c>
@@ -3248,7 +3269,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>10</v>
       </c>
@@ -3268,7 +3289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>230</v>
       </c>
@@ -3288,7 +3309,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>335</v>
       </c>
@@ -3308,7 +3329,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>337</v>
       </c>
@@ -3328,7 +3349,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>93</v>
       </c>
@@ -3348,7 +3369,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>231</v>
       </c>
@@ -3368,7 +3389,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>242</v>
       </c>
@@ -3388,10 +3409,10 @@
         <v>92</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>232</v>
       </c>
@@ -3411,7 +3432,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>334</v>
       </c>
@@ -3431,7 +3452,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>326</v>
       </c>
@@ -3451,7 +3472,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>233</v>
       </c>
@@ -3471,7 +3492,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>330</v>
       </c>
@@ -3491,7 +3512,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>234</v>
       </c>
@@ -3511,7 +3532,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>328</v>
       </c>
@@ -3531,7 +3552,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>332</v>
       </c>
@@ -3551,7 +3572,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>13</v>
       </c>
@@ -3571,7 +3592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -3592,7 +3613,7 @@
       </c>
       <c r="G23" s="33"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -3612,7 +3633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>166</v>
       </c>
@@ -3632,7 +3653,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>160</v>
       </c>
@@ -3652,7 +3673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>139</v>
       </c>
@@ -3672,7 +3693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>164</v>
       </c>
@@ -3692,7 +3713,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>29</v>
       </c>
@@ -3712,7 +3733,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>141</v>
       </c>
@@ -3732,7 +3753,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>127</v>
       </c>
@@ -3752,7 +3773,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
@@ -3772,7 +3793,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>130</v>
       </c>
@@ -3792,7 +3813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
@@ -3812,7 +3833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>176</v>
       </c>
@@ -3832,7 +3853,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
@@ -3852,7 +3873,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>181</v>
       </c>
@@ -3872,7 +3893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>173</v>
       </c>
@@ -3892,7 +3913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>183</v>
       </c>
@@ -3912,7 +3933,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>188</v>
       </c>
@@ -3932,7 +3953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>41</v>
       </c>
@@ -3952,7 +3973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>217</v>
       </c>
@@ -3972,7 +3993,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>136</v>
       </c>
@@ -3992,7 +4013,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>274</v>
       </c>
@@ -4012,10 +4033,10 @@
         <v>44</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>271</v>
       </c>
@@ -4035,10 +4056,10 @@
         <v>44</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>267</v>
       </c>
@@ -4058,10 +4079,10 @@
         <v>44</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>269</v>
       </c>
@@ -4081,10 +4102,10 @@
         <v>44</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>45</v>
       </c>
@@ -4104,10 +4125,10 @@
         <v>44</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>272</v>
       </c>
@@ -4127,10 +4148,10 @@
         <v>44</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>261</v>
       </c>
@@ -4150,10 +4171,10 @@
         <v>44</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>268</v>
       </c>
@@ -4173,10 +4194,10 @@
         <v>44</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>273</v>
       </c>
@@ -4196,10 +4217,10 @@
         <v>44</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>262</v>
       </c>
@@ -4219,10 +4240,10 @@
         <v>44</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>275</v>
       </c>
@@ -4242,10 +4263,10 @@
         <v>44</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>260</v>
       </c>
@@ -4264,11 +4285,11 @@
       <c r="F55" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="G55" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>276</v>
       </c>
@@ -4287,11 +4308,11 @@
       <c r="F56" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G56" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="G56" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>277</v>
       </c>
@@ -4310,11 +4331,11 @@
       <c r="F57" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="G57" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>263</v>
       </c>
@@ -4333,11 +4354,11 @@
       <c r="F58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G58" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="G58" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>278</v>
       </c>
@@ -4357,10 +4378,10 @@
         <v>44</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>48</v>
       </c>
@@ -4380,10 +4401,10 @@
         <v>44</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>50</v>
       </c>
@@ -4403,10 +4424,10 @@
         <v>44</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>52</v>
       </c>
@@ -4426,10 +4447,10 @@
         <v>44</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>266</v>
       </c>
@@ -4448,11 +4469,11 @@
       <c r="F63" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="G63" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>265</v>
       </c>
@@ -4471,11 +4492,11 @@
       <c r="F64" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G64" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="G64" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>264</v>
       </c>
@@ -4494,11 +4515,11 @@
       <c r="F65" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G65" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="G65" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>270</v>
       </c>
@@ -4517,11 +4538,11 @@
       <c r="F66" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G66" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="G66" s="40" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>47</v>
       </c>
@@ -4541,10 +4562,10 @@
         <v>44</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>54</v>
       </c>
@@ -4564,7 +4585,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>229</v>
       </c>
@@ -4584,7 +4605,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>220</v>
       </c>
@@ -4604,7 +4625,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>235</v>
       </c>
@@ -4624,7 +4645,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>226</v>
       </c>
@@ -4644,7 +4665,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>223</v>
       </c>
@@ -4664,7 +4685,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>222</v>
       </c>
@@ -4684,7 +4705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
         <v>156</v>
       </c>
@@ -4704,7 +4725,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
         <v>60</v>
       </c>
@@ -4724,7 +4745,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
         <v>253</v>
       </c>
@@ -4744,7 +4765,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
         <v>153</v>
       </c>
@@ -4764,7 +4785,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
         <v>87</v>
       </c>
@@ -4784,7 +4805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
         <v>148</v>
       </c>
@@ -4804,7 +4825,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>39</v>
       </c>
@@ -4824,7 +4845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>57</v>
       </c>
@@ -4844,7 +4865,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>62</v>
       </c>
@@ -4864,7 +4885,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
         <v>146</v>
       </c>
@@ -4884,7 +4905,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
         <v>316</v>
       </c>
@@ -4904,7 +4925,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
         <v>196</v>
       </c>
@@ -4924,7 +4945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
         <v>204</v>
       </c>
@@ -4944,7 +4965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="s">
         <v>191</v>
       </c>
@@ -4964,7 +4985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
         <v>22</v>
       </c>
@@ -4984,7 +5005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
         <v>206</v>
       </c>
@@ -5004,7 +5025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
         <v>214</v>
       </c>
@@ -5024,7 +5045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
         <v>193</v>
       </c>
@@ -5044,7 +5065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
         <v>216</v>
       </c>
@@ -5064,7 +5085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="s">
         <v>201</v>
       </c>
@@ -5084,7 +5105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="18" t="s">
         <v>210</v>
       </c>
@@ -5104,7 +5125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
         <v>144</v>
       </c>
@@ -5124,7 +5145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>124</v>
       </c>
@@ -5144,7 +5165,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>258</v>
       </c>
@@ -5164,7 +5185,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>104</v>
       </c>
@@ -5184,7 +5205,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>132</v>
       </c>
@@ -5205,7 +5226,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G100">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G100">
     <sortCondition ref="E2:E100"/>
     <sortCondition ref="F2:F100"/>
     <sortCondition ref="B2:B100"/>
@@ -5221,12 +5242,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Abstracted out extensions for curated sources and EVEs
</commit_message>
<xml_diff>
--- a/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/Parvoviridae-GLUE/tabular/references/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC1F8F-68E9-8B4D-AAB1-C9575E7F09D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1123,7 +1117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1286,8 +1280,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="731">
+  <cellStyleXfs count="737">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2062,7 +2062,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="731">
+  <cellStyles count="737">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2428,6 +2428,9 @@
     <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2793,6 +2796,9 @@
     <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3129,14 +3135,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G100"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -3146,7 +3152,7 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
@@ -3209,7 +3215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="35" t="s">
         <v>16</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="37" t="s">
         <v>96</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="37" t="s">
         <v>99</v>
       </c>
@@ -3269,7 +3275,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="30" t="s">
         <v>10</v>
       </c>
@@ -3289,7 +3295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="25" t="s">
         <v>230</v>
       </c>
@@ -3309,7 +3315,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="25" t="s">
         <v>335</v>
       </c>
@@ -3329,7 +3335,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="25" t="s">
         <v>337</v>
       </c>
@@ -3349,7 +3355,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="25" t="s">
         <v>93</v>
       </c>
@@ -3369,7 +3375,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="25" t="s">
         <v>231</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="25" t="s">
         <v>242</v>
       </c>
@@ -3412,7 +3418,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="25" t="s">
         <v>232</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="25" t="s">
         <v>334</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="25" t="s">
         <v>326</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="25" t="s">
         <v>233</v>
       </c>
@@ -3492,7 +3498,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="25" t="s">
         <v>330</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="25" t="s">
         <v>234</v>
       </c>
@@ -3532,7 +3538,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="25" t="s">
         <v>328</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="25" t="s">
         <v>332</v>
       </c>
@@ -3572,7 +3578,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="32" t="s">
         <v>13</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -3613,7 +3619,7 @@
       </c>
       <c r="G23" s="33"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
         <v>166</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="4" t="s">
         <v>160</v>
       </c>
@@ -3673,7 +3679,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="4" t="s">
         <v>139</v>
       </c>
@@ -3693,7 +3699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
         <v>164</v>
       </c>
@@ -3713,7 +3719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="23" t="s">
         <v>29</v>
       </c>
@@ -3733,7 +3739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
         <v>141</v>
       </c>
@@ -3753,7 +3759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="9" t="s">
         <v>127</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="9" t="s">
         <v>130</v>
       </c>
@@ -3813,7 +3819,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
@@ -3833,7 +3839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
         <v>176</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="9" t="s">
         <v>181</v>
       </c>
@@ -3893,7 +3899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
         <v>173</v>
       </c>
@@ -3913,7 +3919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="9" t="s">
         <v>183</v>
       </c>
@@ -3933,7 +3939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
         <v>188</v>
       </c>
@@ -3953,7 +3959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="19" t="s">
         <v>41</v>
       </c>
@@ -3973,7 +3979,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="21" t="s">
         <v>217</v>
       </c>
@@ -3993,7 +3999,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="21" t="s">
         <v>136</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="12" t="s">
         <v>274</v>
       </c>
@@ -4036,7 +4042,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="12" t="s">
         <v>271</v>
       </c>
@@ -4059,7 +4065,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="12" t="s">
         <v>267</v>
       </c>
@@ -4082,7 +4088,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="12" t="s">
         <v>269</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="12" t="s">
         <v>45</v>
       </c>
@@ -4128,7 +4134,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="12" t="s">
         <v>272</v>
       </c>
@@ -4151,7 +4157,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="12" t="s">
         <v>261</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" s="12" t="s">
         <v>268</v>
       </c>
@@ -4197,7 +4203,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
         <v>273</v>
       </c>
@@ -4220,7 +4226,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" s="12" t="s">
         <v>262</v>
       </c>
@@ -4243,7 +4249,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="12" t="s">
         <v>275</v>
       </c>
@@ -4266,7 +4272,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="12" t="s">
         <v>260</v>
       </c>
@@ -4289,7 +4295,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="12" t="s">
         <v>276</v>
       </c>
@@ -4312,7 +4318,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="12" t="s">
         <v>277</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
         <v>263</v>
       </c>
@@ -4358,7 +4364,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="12" t="s">
         <v>278</v>
       </c>
@@ -4381,7 +4387,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="12" t="s">
         <v>48</v>
       </c>
@@ -4404,7 +4410,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" s="12" t="s">
         <v>50</v>
       </c>
@@ -4427,7 +4433,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="12" t="s">
         <v>52</v>
       </c>
@@ -4450,7 +4456,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="12" t="s">
         <v>266</v>
       </c>
@@ -4473,7 +4479,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" s="12" t="s">
         <v>265</v>
       </c>
@@ -4496,7 +4502,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="12" t="s">
         <v>264</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="12" t="s">
         <v>270</v>
       </c>
@@ -4542,7 +4548,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="12" t="s">
         <v>47</v>
       </c>
@@ -4565,7 +4571,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
         <v>54</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
         <v>229</v>
       </c>
@@ -4605,7 +4611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
         <v>220</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
         <v>235</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" s="2" t="s">
         <v>226</v>
       </c>
@@ -4665,7 +4671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
         <v>223</v>
       </c>
@@ -4685,7 +4691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
         <v>222</v>
       </c>
@@ -4705,7 +4711,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" s="14" t="s">
         <v>156</v>
       </c>
@@ -4725,7 +4731,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="14" t="s">
         <v>60</v>
       </c>
@@ -4745,7 +4751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" s="14" t="s">
         <v>253</v>
       </c>
@@ -4765,7 +4771,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" s="14" t="s">
         <v>153</v>
       </c>
@@ -4785,7 +4791,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" s="14" t="s">
         <v>87</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="14" t="s">
         <v>148</v>
       </c>
@@ -4825,7 +4831,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" s="14" t="s">
         <v>39</v>
       </c>
@@ -4845,7 +4851,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" s="14" t="s">
         <v>57</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6">
       <c r="A83" s="14" t="s">
         <v>62</v>
       </c>
@@ -4885,7 +4891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6">
       <c r="A84" s="14" t="s">
         <v>146</v>
       </c>
@@ -4905,7 +4911,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6">
       <c r="A85" s="14" t="s">
         <v>316</v>
       </c>
@@ -4925,7 +4931,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6">
       <c r="A86" s="16" t="s">
         <v>196</v>
       </c>
@@ -4945,7 +4951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" s="16" t="s">
         <v>204</v>
       </c>
@@ -4965,7 +4971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6">
       <c r="A88" s="16" t="s">
         <v>191</v>
       </c>
@@ -4985,7 +4991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" s="16" t="s">
         <v>22</v>
       </c>
@@ -5005,7 +5011,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" s="18" t="s">
         <v>206</v>
       </c>
@@ -5025,7 +5031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" s="18" t="s">
         <v>214</v>
       </c>
@@ -5045,7 +5051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" s="16" t="s">
         <v>193</v>
       </c>
@@ -5065,7 +5071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" s="18" t="s">
         <v>216</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" s="16" t="s">
         <v>201</v>
       </c>
@@ -5105,7 +5111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" s="18" t="s">
         <v>210</v>
       </c>
@@ -5125,7 +5131,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" s="16" t="s">
         <v>144</v>
       </c>
@@ -5145,7 +5151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
         <v>124</v>
       </c>
@@ -5165,7 +5171,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" s="2" t="s">
         <v>258</v>
       </c>
@@ -5185,7 +5191,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" s="2" t="s">
         <v>104</v>
       </c>
@@ -5205,7 +5211,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" s="2" t="s">
         <v>132</v>
       </c>
@@ -5226,7 +5232,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G100">
+  <sortState ref="A2:G100">
     <sortCondition ref="E2:E100"/>
     <sortCondition ref="F2:F100"/>
     <sortCondition ref="B2:B100"/>
@@ -5242,12 +5248,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
More complete dependo extension
</commit_message>
<xml_diff>
--- a/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/references/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E54BE74-B700-C74A-825C-1B3990BC625C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="9820" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="367">
   <si>
     <t>accession-ID</t>
   </si>
@@ -808,9 +814,6 @@
     <t>AF028705</t>
   </si>
   <si>
-    <t>AF085716</t>
-  </si>
-  <si>
     <t>AX753250</t>
   </si>
   <si>
@@ -826,9 +829,6 @@
     <t>AY631966</t>
   </si>
   <si>
-    <t>DI393763</t>
-  </si>
-  <si>
     <t>DQ813647</t>
   </si>
   <si>
@@ -1112,12 +1112,27 @@
   </si>
   <si>
     <t>AAV_primate</t>
+  </si>
+  <si>
+    <t>ChPV-Cebus_imitator.1</t>
+  </si>
+  <si>
+    <t>ChPV-Protobothrops_mucrosquamatus.1</t>
+  </si>
+  <si>
+    <t>ChPV-Serinus_canaria.1</t>
+  </si>
+  <si>
+    <t>ChPV-Mesitornis_unicolor.1</t>
+  </si>
+  <si>
+    <t>ChPV-Myotis_davidii.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3135,14 +3150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B57" sqref="A1:G98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -3152,7 +3167,7 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3172,10 +3187,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -3195,7 +3210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
         <v>16</v>
       </c>
@@ -3235,7 +3250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>96</v>
       </c>
@@ -3255,7 +3270,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>99</v>
       </c>
@@ -3275,7 +3290,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>10</v>
       </c>
@@ -3289,15 +3304,15 @@
         <v>118</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F7" s="31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>230</v>
+        <v>362</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>230</v>
@@ -3309,53 +3324,53 @@
         <v>236</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>107</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>93</v>
       </c>
@@ -3363,21 +3378,21 @@
         <v>91</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>121</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F11" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>231</v>
+        <v>365</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>231</v>
@@ -3389,13 +3404,13 @@
         <v>237</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>242</v>
       </c>
@@ -3409,18 +3424,18 @@
         <v>112</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>232</v>
+        <v>366</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>232</v>
@@ -3432,55 +3447,55 @@
         <v>238</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F14" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D16" s="27" t="s">
         <v>109</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>233</v>
+        <v>363</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>233</v>
@@ -3492,35 +3507,35 @@
         <v>239</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>150</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>234</v>
+        <v>364</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>234</v>
@@ -3532,53 +3547,53 @@
         <v>240</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>246</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>13</v>
       </c>
@@ -3589,16 +3604,16 @@
         <v>84</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F22" s="33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -3609,17 +3624,17 @@
         <v>86</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F23" s="33" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="33"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -3639,7 +3654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>166</v>
       </c>
@@ -3659,7 +3674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>160</v>
       </c>
@@ -3679,7 +3694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>139</v>
       </c>
@@ -3690,7 +3705,7 @@
         <v>137</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>27</v>
@@ -3699,7 +3714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>164</v>
       </c>
@@ -3710,7 +3725,7 @@
         <v>162</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>27</v>
@@ -3719,7 +3734,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>29</v>
       </c>
@@ -3739,7 +3754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>141</v>
       </c>
@@ -3750,7 +3765,7 @@
         <v>140</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>27</v>
@@ -3759,7 +3774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>127</v>
       </c>
@@ -3779,7 +3794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
@@ -3799,7 +3814,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>130</v>
       </c>
@@ -3819,7 +3834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
@@ -3839,7 +3854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>176</v>
       </c>
@@ -3859,7 +3874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
@@ -3879,7 +3894,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>181</v>
       </c>
@@ -3899,7 +3914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>173</v>
       </c>
@@ -3919,7 +3934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>183</v>
       </c>
@@ -3939,7 +3954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>188</v>
       </c>
@@ -3959,7 +3974,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>41</v>
       </c>
@@ -3979,12 +3994,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>217</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>218</v>
@@ -3999,7 +4014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>136</v>
       </c>
@@ -4019,15 +4034,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>114</v>
@@ -4039,18 +4054,18 @@
         <v>44</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>114</v>
@@ -4062,18 +4077,18 @@
         <v>44</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>114</v>
@@ -4085,18 +4100,18 @@
         <v>44</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>114</v>
@@ -4108,10 +4123,10 @@
         <v>44</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>45</v>
       </c>
@@ -4131,18 +4146,18 @@
         <v>44</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>114</v>
@@ -4154,18 +4169,18 @@
         <v>44</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>261</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>114</v>
@@ -4177,18 +4192,18 @@
         <v>44</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D51" s="13" t="s">
         <v>114</v>
@@ -4200,18 +4215,18 @@
         <v>44</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>273</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="D52" s="13" t="s">
         <v>114</v>
@@ -4223,18 +4238,18 @@
         <v>44</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D53" s="13" t="s">
         <v>114</v>
@@ -4245,19 +4260,19 @@
       <c r="F53" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G53" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="G53" s="40" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="D54" s="13" t="s">
         <v>114</v>
@@ -4268,19 +4283,19 @@
       <c r="F54" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="G54" s="40" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>114</v>
@@ -4292,18 +4307,18 @@
         <v>44</v>
       </c>
       <c r="G55" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>114</v>
@@ -4315,18 +4330,18 @@
         <v>44</v>
       </c>
       <c r="G56" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>308</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>309</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>114</v>
@@ -4337,22 +4352,22 @@
       <c r="F57" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G57" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="G57" s="13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>263</v>
+        <v>48</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>285</v>
+        <v>49</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>286</v>
+        <v>71</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>27</v>
@@ -4360,22 +4375,22 @@
       <c r="F58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G58" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="G58" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
-        <v>278</v>
+        <v>50</v>
       </c>
       <c r="B59" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="13" t="s">
         <v>311</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>27</v>
@@ -4384,21 +4399,21 @@
         <v>44</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>178</v>
+        <v>310</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>27</v>
@@ -4407,21 +4422,21 @@
         <v>44</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
-        <v>50</v>
+        <v>265</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>51</v>
+        <v>288</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>313</v>
+        <v>246</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>27</v>
@@ -4429,22 +4444,22 @@
       <c r="F61" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G61" s="40" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>52</v>
+        <v>264</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>53</v>
+        <v>287</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>79</v>
+        <v>290</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>312</v>
+        <v>246</v>
       </c>
       <c r="E62" s="13" t="s">
         <v>27</v>
@@ -4452,19 +4467,19 @@
       <c r="F62" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G62" s="40" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>246</v>
@@ -4476,18 +4491,18 @@
         <v>44</v>
       </c>
       <c r="G63" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="D64" s="13" t="s">
         <v>246</v>
@@ -4499,21 +4514,21 @@
         <v>44</v>
       </c>
       <c r="G64" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
-        <v>264</v>
+        <v>47</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>294</v>
+        <v>90</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>291</v>
+        <v>77</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>246</v>
+        <v>312</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>27</v>
@@ -4521,68 +4536,62 @@
       <c r="F65" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G65" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G66" s="40" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F67" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="G65" s="13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>54</v>
+        <v>220</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>67</v>
+        <v>219</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>114</v>
+        <v>313</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>27</v>
@@ -4591,18 +4600,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>110</v>
+        <v>241</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>27</v>
@@ -4611,18 +4620,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>315</v>
+        <v>227</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>27</v>
@@ -4631,18 +4640,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>27</v>
@@ -4651,18 +4660,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>27</v>
@@ -4671,98 +4680,98 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
-        <v>156</v>
+        <v>253</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>155</v>
+        <v>256</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>154</v>
+        <v>254</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E75" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F75" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E76" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="E76" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F76" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>253</v>
+        <v>87</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>256</v>
+        <v>88</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>254</v>
+        <v>89</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>255</v>
+        <v>113</v>
       </c>
       <c r="E77" s="15" t="s">
         <v>27</v>
@@ -4771,38 +4780,38 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="E78" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E78" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>89</v>
+        <v>349</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>113</v>
+        <v>350</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>27</v>
@@ -4811,18 +4820,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>149</v>
+        <v>58</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E80" s="15" t="s">
         <v>27</v>
@@ -4831,18 +4840,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>351</v>
+        <v>76</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>352</v>
+        <v>109</v>
       </c>
       <c r="E81" s="15" t="s">
         <v>27</v>
@@ -4851,18 +4860,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
-        <v>57</v>
+        <v>146</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>58</v>
+        <v>252</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E82" s="15" t="s">
         <v>27</v>
@@ -4871,15 +4880,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>62</v>
+        <v>314</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>36</v>
+        <v>316</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>76</v>
+        <v>315</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>109</v>
@@ -4891,58 +4900,58 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F85" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>110</v>
+        <v>355</v>
       </c>
       <c r="E86" s="17" t="s">
         <v>27</v>
@@ -4951,18 +4960,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
-        <v>204</v>
+        <v>22</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>202</v>
+        <v>80</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>203</v>
+        <v>111</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>27</v>
@@ -4971,18 +4980,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="16" t="s">
-        <v>191</v>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>357</v>
+        <v>114</v>
       </c>
       <c r="E88" s="17" t="s">
         <v>27</v>
@@ -4991,18 +5000,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="16" t="s">
-        <v>22</v>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C89" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>111</v>
+        <v>213</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>354</v>
       </c>
       <c r="E89" s="17" t="s">
         <v>27</v>
@@ -5011,18 +5020,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="18" t="s">
-        <v>206</v>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>114</v>
+        <v>195</v>
       </c>
       <c r="E90" s="17" t="s">
         <v>27</v>
@@ -5031,18 +5040,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C91" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D91" s="38" t="s">
-        <v>356</v>
+        <v>215</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="E91" s="17" t="s">
         <v>27</v>
@@ -5051,18 +5060,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>27</v>
@@ -5071,18 +5080,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="D93" s="17" t="s">
-        <v>109</v>
+        <v>209</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>353</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>27</v>
@@ -5091,18 +5100,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="s">
-        <v>201</v>
+        <v>144</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>200</v>
+        <v>145</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>199</v>
+        <v>143</v>
       </c>
       <c r="D94" s="17" t="s">
-        <v>109</v>
+        <v>352</v>
       </c>
       <c r="E94" s="17" t="s">
         <v>27</v>
@@ -5111,131 +5120,91 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="C95" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="D95" s="38" t="s">
-        <v>355</v>
-      </c>
-      <c r="E95" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F95" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B96" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C96" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D96" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="E96" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F96" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>353</v>
+        <v>106</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>258</v>
+        <v>132</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>259</v>
+        <v>133</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>257</v>
+        <v>131</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G100">
-    <sortCondition ref="E2:E100"/>
-    <sortCondition ref="F2:F100"/>
-    <sortCondition ref="B2:B100"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G98">
+    <sortCondition ref="E2:E98"/>
+    <sortCondition ref="F2:F98"/>
+    <sortCondition ref="B2:B98"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5248,12 +5217,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Applied new template for comparative/eve projects
</commit_message>
<xml_diff>
--- a/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/references/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/references/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0329A-5904-4B48-A7DE-D844406304BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REFSET" sheetId="3" r:id="rId1"/>
     <sheet name="Minimal refset" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1222,7 +1228,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3571,14 +3577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:G107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
@@ -3588,7 +3594,7 @@
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3631,7 +3637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -3711,7 +3717,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -3751,7 +3757,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -3771,7 +3777,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>333</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>335</v>
       </c>
@@ -3811,7 +3817,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -3831,7 +3837,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>330</v>
       </c>
@@ -3851,7 +3857,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>365</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -3894,7 +3900,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>366</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>332</v>
       </c>
@@ -3934,7 +3940,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>363</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>328</v>
       </c>
@@ -3974,7 +3980,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>370</v>
       </c>
@@ -3994,7 +4000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>364</v>
       </c>
@@ -4014,7 +4020,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -4034,7 +4040,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -4054,7 +4060,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>164</v>
       </c>
@@ -4094,7 +4100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4114,7 +4120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>160</v>
       </c>
@@ -4154,7 +4160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="42" t="s">
         <v>29</v>
       </c>
@@ -4195,7 +4201,7 @@
       </c>
       <c r="G30" s="42"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="42" t="s">
         <v>396</v>
       </c>
@@ -4216,7 +4222,7 @@
       </c>
       <c r="G31" s="42"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
         <v>32</v>
       </c>
@@ -4237,7 +4243,7 @@
       </c>
       <c r="G32" s="43"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="43" t="s">
         <v>130</v>
       </c>
@@ -4258,7 +4264,7 @@
       </c>
       <c r="G33" s="43"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
         <v>37</v>
       </c>
@@ -4279,7 +4285,7 @@
       </c>
       <c r="G34" s="43"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="43" t="s">
         <v>127</v>
       </c>
@@ -4300,7 +4306,7 @@
       </c>
       <c r="G35" s="43"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="s">
         <v>183</v>
       </c>
@@ -4321,7 +4327,7 @@
       </c>
       <c r="G36" s="43"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="s">
         <v>188</v>
       </c>
@@ -4342,7 +4348,7 @@
       </c>
       <c r="G37" s="43"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="43" t="s">
         <v>141</v>
       </c>
@@ -4363,7 +4369,7 @@
       </c>
       <c r="G38" s="43"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="43" t="s">
         <v>173</v>
       </c>
@@ -4384,7 +4390,7 @@
       </c>
       <c r="G39" s="43"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="43" t="s">
         <v>35</v>
       </c>
@@ -4405,7 +4411,7 @@
       </c>
       <c r="G40" s="43"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="43" t="s">
         <v>181</v>
       </c>
@@ -4426,7 +4432,7 @@
       </c>
       <c r="G41" s="43"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="43" t="s">
         <v>176</v>
       </c>
@@ -4447,7 +4453,7 @@
       </c>
       <c r="G42" s="43"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -4467,7 +4473,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>217</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -4507,7 +4513,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>50</v>
       </c>
@@ -4530,7 +4536,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -4553,7 +4559,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>48</v>
       </c>
@@ -4576,7 +4582,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>272</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>269</v>
       </c>
@@ -4622,7 +4628,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>266</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>267</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>45</v>
       </c>
@@ -4691,7 +4697,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>270</v>
       </c>
@@ -4714,7 +4720,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>261</v>
       </c>
@@ -4737,7 +4743,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>271</v>
       </c>
@@ -4760,7 +4766,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>273</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>260</v>
       </c>
@@ -4806,7 +4812,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>274</v>
       </c>
@@ -4829,7 +4835,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>275</v>
       </c>
@@ -4852,7 +4858,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>262</v>
       </c>
@@ -4875,7 +4881,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>276</v>
       </c>
@@ -4898,7 +4904,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>265</v>
       </c>
@@ -4921,7 +4927,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>264</v>
       </c>
@@ -4944,7 +4950,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>263</v>
       </c>
@@ -4967,7 +4973,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>268</v>
       </c>
@@ -4990,7 +4996,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>368</v>
       </c>
@@ -5011,7 +5017,7 @@
       </c>
       <c r="G67" s="12"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>369</v>
       </c>
@@ -5032,7 +5038,7 @@
       </c>
       <c r="G68" s="12"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
         <v>47</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>378</v>
       </c>
@@ -5074,7 +5080,7 @@
       </c>
       <c r="G70" s="12"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="12" t="s">
         <v>379</v>
       </c>
@@ -5093,7 +5099,7 @@
       </c>
       <c r="G71" s="12"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="12" t="s">
         <v>380</v>
       </c>
@@ -5112,7 +5118,7 @@
       </c>
       <c r="G72" s="12"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>381</v>
       </c>
@@ -5131,7 +5137,7 @@
       </c>
       <c r="G73" s="12"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>382</v>
       </c>
@@ -5150,7 +5156,7 @@
       </c>
       <c r="G74" s="12"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>383</v>
       </c>
@@ -5169,7 +5175,7 @@
       </c>
       <c r="G75" s="12"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>229</v>
       </c>
@@ -5189,7 +5195,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>367</v>
       </c>
@@ -5209,7 +5215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>54</v>
       </c>
@@ -5229,7 +5235,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>226</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>222</v>
       </c>
@@ -5269,7 +5275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>223</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>220</v>
       </c>
@@ -5309,7 +5315,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>60</v>
       </c>
@@ -5329,7 +5335,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -5349,7 +5355,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>39</v>
       </c>
@@ -5369,7 +5375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>253</v>
       </c>
@@ -5389,7 +5395,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>156</v>
       </c>
@@ -5409,7 +5415,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>153</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>57</v>
       </c>
@@ -5449,7 +5455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>148</v>
       </c>
@@ -5469,7 +5475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>62</v>
       </c>
@@ -5489,7 +5495,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>146</v>
       </c>
@@ -5509,7 +5515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>314</v>
       </c>
@@ -5529,7 +5535,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>210</v>
       </c>
@@ -5549,7 +5555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>144</v>
       </c>
@@ -5569,7 +5575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -5589,7 +5595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -5609,7 +5615,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -5629,7 +5635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -5649,7 +5655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>191</v>
       </c>
@@ -5669,7 +5675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>193</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -5709,7 +5715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>216</v>
       </c>
@@ -5729,7 +5735,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>201</v>
       </c>
@@ -5749,7 +5755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>132</v>
       </c>
@@ -5769,7 +5775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -5789,7 +5795,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>124</v>
       </c>
@@ -5810,7 +5816,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G106">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G106">
     <sortCondition ref="E2:E106"/>
     <sortCondition ref="F2:F106"/>
     <sortCondition ref="D2:D106"/>
@@ -5826,14 +5832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -5843,7 +5849,7 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5866,7 +5872,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -5886,7 +5892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
@@ -5906,7 +5912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
         <v>16</v>
       </c>
@@ -5926,7 +5932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>96</v>
       </c>
@@ -5946,7 +5952,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>99</v>
       </c>
@@ -5966,7 +5972,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>10</v>
       </c>
@@ -5986,7 +5992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>362</v>
       </c>
@@ -6006,7 +6012,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>333</v>
       </c>
@@ -6026,7 +6032,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>335</v>
       </c>
@@ -6046,7 +6052,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>93</v>
       </c>
@@ -6066,7 +6072,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>365</v>
       </c>
@@ -6086,7 +6092,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>242</v>
       </c>
@@ -6109,7 +6115,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>366</v>
       </c>
@@ -6129,7 +6135,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>332</v>
       </c>
@@ -6149,7 +6155,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>324</v>
       </c>
@@ -6169,7 +6175,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>363</v>
       </c>
@@ -6189,7 +6195,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>328</v>
       </c>
@@ -6209,7 +6215,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>364</v>
       </c>
@@ -6229,7 +6235,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>326</v>
       </c>
@@ -6249,7 +6255,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>330</v>
       </c>
@@ -6269,7 +6275,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>370</v>
       </c>
@@ -6289,7 +6295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>13</v>
       </c>
@@ -6309,7 +6315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>19</v>
       </c>
@@ -6330,7 +6336,7 @@
       </c>
       <c r="G24" s="33"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -6350,7 +6356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>166</v>
       </c>
@@ -6370,7 +6376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>160</v>
       </c>
@@ -6390,7 +6396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>139</v>
       </c>
@@ -6410,7 +6416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>164</v>
       </c>
@@ -6430,7 +6436,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>29</v>
       </c>
@@ -6450,7 +6456,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>141</v>
       </c>
@@ -6470,7 +6476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>127</v>
       </c>
@@ -6490,7 +6496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -6510,7 +6516,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>130</v>
       </c>
@@ -6530,7 +6536,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>37</v>
       </c>
@@ -6550,7 +6556,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>176</v>
       </c>
@@ -6570,7 +6576,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>35</v>
       </c>
@@ -6590,7 +6596,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>181</v>
       </c>
@@ -6610,7 +6616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>173</v>
       </c>
@@ -6630,7 +6636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>183</v>
       </c>
@@ -6650,7 +6656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>188</v>
       </c>
@@ -6670,7 +6676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>41</v>
       </c>
@@ -6690,7 +6696,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>217</v>
       </c>
@@ -6710,7 +6716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>136</v>
       </c>
@@ -6730,7 +6736,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>272</v>
       </c>
@@ -6753,7 +6759,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>269</v>
       </c>
@@ -6776,7 +6782,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>266</v>
       </c>
@@ -6799,7 +6805,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>267</v>
       </c>
@@ -6822,7 +6828,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>45</v>
       </c>
@@ -6845,7 +6851,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>270</v>
       </c>
@@ -6868,7 +6874,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>261</v>
       </c>
@@ -6891,7 +6897,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>271</v>
       </c>
@@ -6914,7 +6920,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>273</v>
       </c>
@@ -6937,7 +6943,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>260</v>
       </c>
@@ -6960,7 +6966,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>274</v>
       </c>
@@ -6983,7 +6989,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>275</v>
       </c>
@@ -7006,7 +7012,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>262</v>
       </c>
@@ -7029,7 +7035,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>276</v>
       </c>
@@ -7052,7 +7058,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>48</v>
       </c>
@@ -7075,7 +7081,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>50</v>
       </c>
@@ -7098,7 +7104,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>52</v>
       </c>
@@ -7121,7 +7127,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>265</v>
       </c>
@@ -7144,7 +7150,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>264</v>
       </c>
@@ -7167,7 +7173,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>263</v>
       </c>
@@ -7190,7 +7196,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>268</v>
       </c>
@@ -7213,7 +7219,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>47</v>
       </c>
@@ -7236,7 +7242,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>368</v>
       </c>
@@ -7257,7 +7263,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>369</v>
       </c>
@@ -7278,7 +7284,7 @@
       </c>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>54</v>
       </c>
@@ -7298,7 +7304,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>229</v>
       </c>
@@ -7318,7 +7324,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>220</v>
       </c>
@@ -7338,7 +7344,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>367</v>
       </c>
@@ -7358,7 +7364,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>226</v>
       </c>
@@ -7378,7 +7384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>223</v>
       </c>
@@ -7398,7 +7404,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>222</v>
       </c>
@@ -7418,7 +7424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
         <v>156</v>
       </c>
@@ -7438,7 +7444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
         <v>60</v>
       </c>
@@ -7458,7 +7464,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
         <v>253</v>
       </c>
@@ -7478,7 +7484,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
         <v>153</v>
       </c>
@@ -7498,7 +7504,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
         <v>87</v>
       </c>
@@ -7518,7 +7524,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>148</v>
       </c>
@@ -7538,7 +7544,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>39</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>57</v>
       </c>
@@ -7578,7 +7584,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
         <v>62</v>
       </c>
@@ -7598,7 +7604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
         <v>146</v>
       </c>
@@ -7618,7 +7624,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
         <v>314</v>
       </c>
@@ -7638,7 +7644,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
         <v>196</v>
       </c>
@@ -7658,7 +7664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="s">
         <v>204</v>
       </c>
@@ -7678,7 +7684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
         <v>191</v>
       </c>
@@ -7698,7 +7704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="16" t="s">
         <v>22</v>
       </c>
@@ -7718,7 +7724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
         <v>206</v>
       </c>
@@ -7738,7 +7744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="18" t="s">
         <v>214</v>
       </c>
@@ -7758,7 +7764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
         <v>193</v>
       </c>
@@ -7778,7 +7784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="18" t="s">
         <v>216</v>
       </c>
@@ -7798,7 +7804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="s">
         <v>201</v>
       </c>
@@ -7818,7 +7824,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="18" t="s">
         <v>210</v>
       </c>
@@ -7838,7 +7844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="s">
         <v>144</v>
       </c>
@@ -7858,7 +7864,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>124</v>
       </c>
@@ -7878,7 +7884,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>258</v>
       </c>
@@ -7898,7 +7904,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>104</v>
       </c>
@@ -7918,7 +7924,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>132</v>
       </c>
@@ -7938,7 +7944,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
         <v>378</v>
       </c>
@@ -7956,7 +7962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>379</v>
       </c>
@@ -7974,7 +7980,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
         <v>380</v>
       </c>
@@ -7992,7 +7998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>381</v>
       </c>
@@ -8010,7 +8016,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
         <v>382</v>
       </c>
@@ -8028,7 +8034,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
         <v>383</v>
       </c>
@@ -8047,7 +8053,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G98">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G98">
     <sortCondition ref="E2:E98"/>
     <sortCondition ref="F2:F98"/>
     <sortCondition ref="B2:B98"/>

</xml_diff>